<commit_message>
Modify Clean Data to new setting
</commit_message>
<xml_diff>
--- a/results/table1/coh_1.xlsx
+++ b/results/table1/coh_1.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,10 +519,10 @@
       <c r="B4" s="1" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>2448</v>
+        <v>5509</v>
       </c>
       <c r="E4" t="n">
-        <v>10603</v>
+        <v>11090</v>
       </c>
     </row>
     <row r="5">
@@ -541,12 +541,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1015 (41.5)</t>
+          <t>1528 (27.7)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3965 (37.4)</t>
+          <t>4208 (37.9)</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>596 (24.3)</t>
+          <t>1335 (24.2)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2561 (24.2)</t>
+          <t>2672 (24.1)</t>
         </is>
       </c>
     </row>
@@ -579,12 +579,12 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>507 (20.7)</t>
+          <t>1453 (26.4)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2420 (22.8)</t>
+          <t>2494 (22.5)</t>
         </is>
       </c>
     </row>
@@ -598,12 +598,12 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>330 (13.5)</t>
+          <t>1193 (21.7)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1657 (15.6)</t>
+          <t>1716 (15.5)</t>
         </is>
       </c>
     </row>
@@ -623,12 +623,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1170 (47.8)</t>
+          <t>2357 (42.8)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4450 (42.0)</t>
+          <t>4654 (42.0)</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>932 (38.1)</t>
+          <t>2175 (39.5)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5370 (50.6)</t>
+          <t>5630 (50.8)</t>
         </is>
       </c>
     </row>
@@ -667,12 +667,12 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>342 (14.0)</t>
+          <t>624 (11.3)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>560 (5.3)</t>
+          <t>591 (5.3)</t>
         </is>
       </c>
     </row>
@@ -686,12 +686,12 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1174 (48.0)</t>
+          <t>2710 (49.2)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4673 (44.1)</t>
+          <t>4869 (43.9)</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>770 (31.5)</t>
+          <t>1232 (22.4)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>490 (4.6)</t>
+          <t>515 (4.6)</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>196 (8.0)</t>
+          <t>408 (7.4)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1545 (14.6)</t>
+          <t>1573 (14.2)</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>805 (32.9)</t>
+          <t>1903 (34.5)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4481 (42.3)</t>
+          <t>4633 (41.8)</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>434 (17.7)</t>
+          <t>1308 (23.7)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1762 (16.6)</t>
+          <t>2075 (18.7)</t>
         </is>
       </c>
     </row>
@@ -811,19 +811,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>650 (26.6)</t>
+          <t>1716 (31.1)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2667 (25.2)</t>
+          <t>3048 (27.5)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Mechanical Ventilation (whole stay), n (%)</t>
+          <t>MV initiated until the cohort day, n (%)</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
@@ -836,19 +836,19 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1392 (56.9)</t>
+          <t>3230 (58.6)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6318 (59.6)</t>
+          <t>5698 (51.4)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>RRT (whole stay), n (%)</t>
+          <t>RRT initiated until the cohort day, n (%)</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
@@ -861,19 +861,19 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>371 (15.2)</t>
+          <t>451 (8.2)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1027 (9.7)</t>
+          <t>540 (4.9)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Vasopressors (whole stay), n (%)</t>
+          <t>Vasopressor initiated until the cohort day, n (%)</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
@@ -886,24 +886,24 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1181 (48.2)</t>
+          <t>2555 (46.4)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5932 (55.9)</t>
+          <t>5333 (48.1)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Insulin Transfusion (whole stay), n (%)</t>
+          <t>Mechanical Ventilation (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -911,24 +911,24 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1502 (61.4)</t>
+          <t>3675 (66.7)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6318 (59.6)</t>
+          <t>6715 (60.6)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Blood Transufusion (whole stay), n (%)</t>
+          <t>RRT (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -936,24 +936,24 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>256 (10.5)</t>
+          <t>824 (15.0)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1296 (12.2)</t>
+          <t>1159 (10.5)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Fluids Received (whole stay), n (%)</t>
+          <t>Vasopressors (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -961,19 +961,19 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2385 (97.4)</t>
+          <t>3049 (55.3)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>10357 (97.7)</t>
+          <t>6313 (56.9)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Hypertension, n (%)</t>
+          <t>Insulin Transfusion (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
@@ -986,19 +986,19 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1704 (69.6)</t>
+          <t>3379 (61.3)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6977 (65.8)</t>
+          <t>6677 (60.2)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Congestive Heart Failure, n (%)</t>
+          <t>Blood Transufusion (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
@@ -1011,19 +1011,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>915 (37.4)</t>
+          <t>641 (11.6)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3851 (36.3)</t>
+          <t>1368 (12.3)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>COPD, n (%)</t>
+          <t>Fluids Received (whole stay), n (%)</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
@@ -1036,19 +1036,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>562 (23.0)</t>
+          <t>5398 (98.0)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2623 (24.7)</t>
+          <t>10844 (97.8)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Asthma, n (%)</t>
+          <t>Hypertension, n (%)</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
@@ -1061,19 +1061,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>34 (1.4)</t>
+          <t>3571 (64.8)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>152 (1.4)</t>
+          <t>7269 (65.5)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Coronary Artery Disease, n (%)</t>
+          <t>Congestive Heart Failure, n (%)</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
@@ -1086,94 +1086,112 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>754 (30.8)</t>
+          <t>1887 (34.3)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4137 (39.0)</t>
+          <t>4054 (36.6)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
+          <t>COPD, n (%)</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1259 (22.9)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2748 (24.8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Asthma, n (%)</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>66 (1.2)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>171 (1.5)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Coronary Artery Disease, n (%)</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1810 (32.9)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>4304 (38.8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
           <t>CKD Stage, n (%)</t>
         </is>
       </c>
-      <c r="B29" s="1" t="inlineStr">
+      <c r="B32" s="1" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>3 (0.1)</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>4 (0.1)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>2 (0.0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>19 (0.8)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>68 (0.6)</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>161 (6.6)</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>532 (5.0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>62 (2.5)</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>185 (1.7)</t>
         </is>
       </c>
     </row>
@@ -1181,18 +1199,18 @@
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>264 (10.8)</t>
+          <t>32 (0.6)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>461 (4.3)</t>
+          <t>70 (0.6)</t>
         </is>
       </c>
     </row>
@@ -1200,43 +1218,37 @@
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1939 (79.2)</t>
+          <t>294 (5.3)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>9355 (88.2)</t>
+          <t>549 (5.0)</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Diabetes Type, n (%)</t>
-        </is>
-      </c>
+      <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>75 (3.1)</t>
+          <t>103 (1.9)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>300 (2.8)</t>
+          <t>196 (1.8)</t>
         </is>
       </c>
     </row>
@@ -1244,18 +1256,18 @@
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>986 (40.3)</t>
+          <t>395 (7.2)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2962 (27.9)</t>
+          <t>486 (4.4)</t>
         </is>
       </c>
     </row>
@@ -1269,19 +1281,19 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1387 (56.7)</t>
+          <t>4681 (85.0)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7341 (69.2)</t>
+          <t>9787 (88.3)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Connective Tissue Disease, n (%)</t>
+          <t>Diabetes Type, n (%)</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
@@ -1294,69 +1306,57 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>117 (4.8)</t>
+          <t>127 (2.3)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>472 (4.5)</t>
+          <t>312 (2.8)</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Pneumonia, n (%)</t>
-        </is>
-      </c>
+      <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>139 (5.7)</t>
+          <t>1844 (33.5)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>507 (4.8)</t>
+          <t>3084 (27.8)</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Urinary Tract Infection, n (%)</t>
-        </is>
-      </c>
+      <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15 (0.6)</t>
+          <t>3538 (64.2)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>84 (0.8)</t>
+          <t>7694 (69.4)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Biliary Tract Infection, n (%)</t>
+          <t>Connective Tissue Disease, n (%)</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr">
@@ -1369,19 +1369,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2 (0.1)</t>
+          <t>225 (4.1)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>20 (0.2)</t>
+          <t>496 (4.5)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Skin Infection, n (%)</t>
+          <t>Pneumonia, n (%)</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr">
@@ -1394,24 +1394,24 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4 (0.2)</t>
+          <t>305 (5.5)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>21 (0.2)</t>
+          <t>523 (4.7)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>MV_elig_day, n (%)</t>
+          <t>Urinary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1419,24 +1419,24 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1214 (49.6)</t>
+          <t>31 (0.6)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>5432 (51.2)</t>
+          <t>88 (0.8)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>RRT_elig_day, n (%)</t>
+          <t>Biliary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1444,24 +1444,24 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>233 (9.5)</t>
+          <t>9 (0.2)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>507 (4.8)</t>
+          <t>23 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>VP_elig_day, n (%)</t>
+          <t>Skin Infection, n (%)</t>
         </is>
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1469,1276 +1469,976 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1004 (41.0)</t>
+          <t>6 (0.1)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5094 (48.0)</t>
+          <t>21 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>MV initiated in day 1, n (%)</t>
-        </is>
-      </c>
-      <c r="B46" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>Age, median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr"/>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1207 (49.3)</t>
+          <t>64 [52,76]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>5398 (50.9)</t>
+          <t>68 [58,79]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>RRT initiated in day 1, n (%)</t>
-        </is>
-      </c>
-      <c r="B47" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr"/>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>13216</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>227 (9.3)</t>
+          <t>5.79 [3.58,10.68]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>494 (4.7)</t>
+          <t>5.79 [3.54,10.29]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor initiated in day 1, n (%)</t>
-        </is>
-      </c>
-      <c r="B48" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr"/>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>3383</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>999 (40.8)</t>
+          <t>4.63 [2.96,9.00]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5074 (47.9)</t>
+          <t>4.13 [2.83,7.46]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>MV initiated in day 2, n (%)</t>
-        </is>
-      </c>
-      <c r="B49" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>Hospital LOS (days, if deceased), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr"/>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>13216</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>75 (3.1)</t>
+          <t>9.00 [5.00,18.00]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>423 (4.0)</t>
+          <t>11.00 [6.00,19.00]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>RRT initiated in day 2, n (%)</t>
-        </is>
-      </c>
-      <c r="B50" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>Hospital LOS (days, if survived), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr"/>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>3383</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>59 (2.4)</t>
+          <t>12.00 [7.00,20.00]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>198 (1.9)</t>
+          <t>11.00 [7.00,18.00]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor initiated in day 2, n (%)</t>
-        </is>
-      </c>
-      <c r="B51" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr"/>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>78 (3.2)</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>392 (3.7)</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>MV initiated in day 3, n (%)</t>
-        </is>
-      </c>
-      <c r="B52" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>SOFA Score (admission), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr"/>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>39 (1.6)</t>
+          <t>6 [4,9]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>216 (2.0)</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>RRT initiated in day 3, n (%)</t>
-        </is>
-      </c>
-      <c r="B53" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>SOFA: Respiratory (admission), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr"/>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>5621</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>30 (1.2)</t>
+          <t>2 [1,3]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>120 (1.1)</t>
+          <t>2 [1,3]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor initiated in day 3, n (%)</t>
-        </is>
-      </c>
-      <c r="B54" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>SOFA: Coagulation (admission), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr"/>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>37 (1.5)</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>197 (1.9)</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>MV initiated in day 4, n (%)</t>
-        </is>
-      </c>
-      <c r="B55" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>SOFA: Liver (admission), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr"/>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>6262</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>31 (1.3)</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>106 (1.0)</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>RRT initiated in day 4, n (%)</t>
-        </is>
-      </c>
-      <c r="B56" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>SOFA: Cardiovascular (admission), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr"/>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>17 (0.7)</t>
+          <t>1 [1,4]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>57 (0.5)</t>
+          <t>1 [1,3]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor initiated in day 4, n (%)</t>
-        </is>
-      </c>
-      <c r="B57" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>SOFA: CNS (admission), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr"/>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>27 (1.1)</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>99 (0.9)</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Age, median [Q1,Q3]</t>
+          <t>SOFA: Renal (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B58" s="1" t="inlineStr"/>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>64 [52,75]</t>
+          <t>1 [0,2]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>68 [58,78]</t>
+          <t>1 [0,2]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
+          <t>sofa_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B59" s="1" t="inlineStr"/>
       <c r="C59" t="n">
-        <v>10855</v>
+        <v>16</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5.23 [3.23,8.99]</t>
+          <t>5.0 [3.0,8.0]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5.38 [3.29,9.38]</t>
+          <t>5.0 [3.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
+          <t>respiratory_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B60" s="1" t="inlineStr"/>
       <c r="C60" t="n">
-        <v>2196</v>
+        <v>16</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4.17 [2.83,7.71]</t>
+          <t>1.0 [0.0,2.0]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>4.08 [2.79,7.17]</t>
+          <t>1.0 [0.0,2.0]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Hospital LOS (days, if deceased), median [Q1,Q3]</t>
+          <t>coagulation_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B61" s="1" t="inlineStr"/>
       <c r="C61" t="n">
-        <v>10855</v>
+        <v>16</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>10.00 [6.00,19.00]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>11.00 [6.00,18.75]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Hospital LOS (days, if survived), median [Q1,Q3]</t>
+          <t>liver_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B62" s="1" t="inlineStr"/>
       <c r="C62" t="n">
-        <v>2196</v>
+        <v>16</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12.00 [7.00,20.00]</t>
+          <t>0.0 [0.0,0.0]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>11.00 [7.00,18.00]</t>
+          <t>0.0 [0.0,0.0]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
+          <t>cardiovascular_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B63" s="1" t="inlineStr"/>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>1.0 [1.0,3.0]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>1.0 [1.0,3.0]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>SOFA Score (admission), median [Q1,Q3]</t>
+          <t>cns_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B64" s="1" t="inlineStr"/>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5 [3,8]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Respiratory (admission), median [Q1,Q3]</t>
+          <t>renal_max_0_24h, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B65" s="1" t="inlineStr"/>
       <c r="C65" t="n">
-        <v>4756</v>
+        <v>16</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2 [1,3]</t>
+          <t>1.0 [0.0,2.0]</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2 [1,3]</t>
+          <t>0.0 [0.0,1.0]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Coagulation (admission), median [Q1,Q3]</t>
+          <t>Fluids Volume (first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B66" s="1" t="inlineStr"/>
       <c r="C66" t="n">
-        <v>28</v>
+        <v>5744</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>800 [250,1564]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>681 [221,1500]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Liver (admission), median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B67" s="1" t="inlineStr"/>
       <c r="C67" t="n">
-        <v>5163</v>
+        <v>357</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>3304 [1158,7044]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>2546 [869,5885]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Cardiovascular (admission), median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B68" s="1" t="inlineStr"/>
       <c r="C68" t="n">
-        <v>18</v>
+        <v>357</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1 [1,3]</t>
+          <t>549.5 [259.8,1016.1]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1 [1,3]</t>
+          <t>487.9 [213.9,917.0]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>SOFA: CNS (admission), median [Q1,Q3]</t>
+          <t>FiO2 (mean %, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B69" s="1" t="inlineStr"/>
       <c r="C69" t="n">
-        <v>22</v>
+        <v>9234</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>50 [40,62]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>50 [42,65]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Renal (admission), median [Q1,Q3]</t>
+          <t>MV_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B70" s="1" t="inlineStr"/>
       <c r="C70" t="n">
-        <v>1</v>
+        <v>6209</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1 [0,2]</t>
+          <t>45.0 [18.0,98.0]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1 [0,2]</t>
+          <t>35.0 [15.0,86.0]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>SOFA (day), median [Q1,Q3]</t>
+          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B71" s="1" t="inlineStr"/>
       <c r="C71" t="n">
-        <v>15</v>
+        <v>6209</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>5.0 [3.0,8.0]</t>
+          <t>0.31 [0.15,0.53]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>5.0 [3.0,8.0]</t>
+          <t>0.27 [0.13,0.46]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Respiratory (day), median [Q1,Q3]</t>
+          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B72" s="1" t="inlineStr"/>
       <c r="C72" t="n">
-        <v>15</v>
+        <v>6209</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.0 [0.0,2.0]</t>
+          <t>2.0 [1.0,6.0]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>3.0 [1.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Coagulation (day), median [Q1,Q3]</t>
+          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B73" s="1" t="inlineStr"/>
       <c r="C73" t="n">
-        <v>15</v>
+        <v>14616</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>20.0 [4.0,58.2]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>27.0 [6.0,69.0]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Liver (day), median [Q1,Q3]</t>
+          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B74" s="1" t="inlineStr"/>
       <c r="C74" t="n">
-        <v>15</v>
+        <v>7088</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.0 [0.0,0.0]</t>
+          <t>3.0 [1.0,12.0]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.0 [0.0,0.0]</t>
+          <t>3.0 [1.0,10.0]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Cardiovascular (day), median [Q1,Q3]</t>
+          <t>VP_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B75" s="1" t="inlineStr"/>
       <c r="C75" t="n">
-        <v>15</v>
+        <v>7088</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.0 [1.0,3.0]</t>
+          <t>34.0 [12.0,80.0]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1.0 [1.0,3.0]</t>
+          <t>31.0 [11.0,68.0]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>SOFA: CNS (day), median [Q1,Q3]</t>
+          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B76" s="1" t="inlineStr"/>
       <c r="C76" t="n">
-        <v>15</v>
+        <v>7088</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>0.26 [0.09,0.52]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>0.25 [0.09,0.48]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Renal (day), median [Q1,Q3]</t>
+          <t>Respiratory Rate (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B77" s="1" t="inlineStr"/>
       <c r="C77" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>19.4 [17.0,22.5]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>19.1 [16.8,22.1]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (day), median [Q1,Q3]</t>
+          <t>Mean Blood Pressure (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B78" s="1" t="inlineStr"/>
       <c r="C78" t="n">
-        <v>4731</v>
+        <v>22</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>729 [246,1498]</t>
+          <t>76.7 [70.8,84.4]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>650 [210,1463]</t>
+          <t>74.7 [69.4,81.5]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
+          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B79" s="1" t="inlineStr"/>
       <c r="C79" t="n">
-        <v>309</v>
+        <v>899</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2648 [994,5920]</t>
+          <t>36.9 [36.6,37.3]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2369 [817,5431]</t>
+          <t>36.9 [36.6,37.2]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
+          <t>SpO2 (%, mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B80" s="1" t="inlineStr"/>
       <c r="C80" t="n">
-        <v>309</v>
+        <v>24</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>506.2 [226.7,963.1]</t>
+          <t>97.8 [96.2,99.0]</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>477.0 [204.8,905.2]</t>
+          <t>97.2 [95.8,98.6]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>FiO2 (mean %), median [Q1,Q3]</t>
+          <t>Heart Rate (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B81" s="1" t="inlineStr"/>
       <c r="C81" t="n">
-        <v>7672</v>
+        <v>22</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>50 [40,60]</t>
+          <t>86.7 [76.2,99.5]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>50 [42,65]</t>
+          <t>86.0 [75.9,98.2]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>MV_time_abs_hours, median [Q1,Q3]</t>
+          <t>PaO2 (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B82" s="1" t="inlineStr"/>
       <c r="C82" t="n">
-        <v>5341</v>
+        <v>4762</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>39.0 [17.0,86.2]</t>
+          <t>88.0 [70.0,123.0]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>32.0 [15.0,76.0]</t>
+          <t>88.0 [71.0,117.0]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>PaCO2 (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B83" s="1" t="inlineStr"/>
       <c r="C83" t="n">
-        <v>5341</v>
+        <v>4762</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0.30 [0.14,0.50]</t>
+          <t>44.0 [38.0,52.0]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>0.26 [0.13,0.45]</t>
+          <t>46.0 [39.0,53.0]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>pH (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B84" s="1" t="inlineStr"/>
       <c r="C84" t="n">
-        <v>5341</v>
+        <v>2649</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2.0 [1.0,8.0]</t>
+          <t>7.3 [7.2,7.4]</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>3.0 [1.0,8.0]</t>
+          <t>7.3 [7.2,7.4]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>Glucose (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B85" s="1" t="inlineStr"/>
       <c r="C85" t="n">
-        <v>11653</v>
+        <v>82</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>16.0 [4.0,41.0]</t>
+          <t>154.0 [123.0,209.0]</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>25.0 [5.5,63.0]</t>
+          <t>147.0 [120.0,194.0]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>Sodium (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B86" s="1" t="inlineStr"/>
       <c r="C86" t="n">
-        <v>5827</v>
+        <v>33</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>3.0 [1.0,12.0]</t>
+          <t>137.0 [134.0,140.0]</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>3.0 [1.0,10.0]</t>
+          <t>137.0 [134.0,140.0]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>VP_time_abs_hours, median [Q1,Q3]</t>
+          <t>Potassium (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B87" s="1" t="inlineStr"/>
       <c r="C87" t="n">
-        <v>5827</v>
+        <v>40</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>29.0 [10.0,65.0]</t>
+          <t>4.5 [4.1,5.1]</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>29.0 [11.0,62.0]</t>
+          <t>4.5 [4.1,5.0]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>Cortisol (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B88" s="1" t="inlineStr"/>
       <c r="C88" t="n">
-        <v>5827</v>
+        <v>16187</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>0.23 [0.08,0.48]</t>
+          <t>22.6 [14.2,35.0]</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>0.25 [0.09,0.47]</t>
+          <t>22.4 [12.5,35.5]</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>Respiratory Rate (mean), median [Q1,Q3]</t>
+          <t>Hemoglobin (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B89" s="1" t="inlineStr"/>
       <c r="C89" t="n">
-        <v>24</v>
+        <v>2238</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>19.4 [17.0,22.6]</t>
+          <t>10.0 [8.5,11.7]</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>19.1 [16.8,22.0]</t>
+          <t>10.0 [8.6,11.6]</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>Mean Blood Pressure (mean), median [Q1,Q3]</t>
+          <t>Fibrinogen (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B90" s="1" t="inlineStr"/>
       <c r="C90" t="n">
-        <v>18</v>
+        <v>10497</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>77.5 [71.1,85.4]</t>
+          <t>229.0 [159.0,346.0]</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>74.7 [69.4,81.6]</t>
+          <t>230.0 [165.0,349.0]</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
+          <t>INR (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B91" s="1" t="inlineStr"/>
       <c r="C91" t="n">
-        <v>693</v>
+        <v>899</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.3]</t>
+          <t>1.3 [1.2,1.7]</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
-        <is>
-          <t>36.9 [36.6,37.2]</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>SpO2 (%, mean), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B92" s="1" t="inlineStr"/>
-      <c r="C92" t="n">
-        <v>19</v>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>98.0 [96.3,99.2]</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>97.2 [95.8,98.6]</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="inlineStr">
-        <is>
-          <t>Heart Rate (mean), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B93" s="1" t="inlineStr"/>
-      <c r="C93" t="n">
-        <v>18</v>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>87.5 [76.4,100.6]</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>85.8 [75.8,97.9]</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>PaO2 (min), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B94" s="1" t="inlineStr"/>
-      <c r="C94" t="n">
-        <v>4014</v>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>88.5 [69.0,124.0]</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>89.0 [72.0,118.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="inlineStr">
-        <is>
-          <t>PaCO2 (max), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B95" s="1" t="inlineStr"/>
-      <c r="C95" t="n">
-        <v>4014</v>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>44.0 [37.0,52.0]</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>46.0 [39.0,53.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="inlineStr">
-        <is>
-          <t>pH (min), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B96" s="1" t="inlineStr"/>
-      <c r="C96" t="n">
-        <v>2267</v>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>7.3 [7.2,7.4]</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>7.3 [7.2,7.4]</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="inlineStr">
-        <is>
-          <t>Glucose (max), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B97" s="1" t="inlineStr"/>
-      <c r="C97" t="n">
-        <v>67</v>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>154.0 [122.0,218.0]</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>147.0 [120.0,194.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>Sodium (min), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B98" s="1" t="inlineStr"/>
-      <c r="C98" t="n">
-        <v>27</v>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>137.0 [134.0,140.0]</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>137.0 [134.0,140.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="inlineStr">
-        <is>
-          <t>Potassium (max), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B99" s="1" t="inlineStr"/>
-      <c r="C99" t="n">
-        <v>34</v>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>4.5 [4.1,5.2]</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>4.5 [4.1,5.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="inlineStr">
-        <is>
-          <t>Cortisol (min), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B100" s="1" t="inlineStr"/>
-      <c r="C100" t="n">
-        <v>12719</v>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>19.0 [13.5,30.9]</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>22.0 [12.5,33.9]</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="inlineStr">
-        <is>
-          <t>Hemoglobin (min), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B101" s="1" t="inlineStr"/>
-      <c r="C101" t="n">
-        <v>1753</v>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>9.8 [8.2,11.4]</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>10.0 [8.6,11.6]</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="inlineStr">
-        <is>
-          <t>Fibrinogen (min), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B102" s="1" t="inlineStr"/>
-      <c r="C102" t="n">
-        <v>8424</v>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>226.0 [153.0,364.0]</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>228.5 [165.0,344.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="inlineStr">
-        <is>
-          <t>INR (max), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B103" s="1" t="inlineStr"/>
-      <c r="C103" t="n">
-        <v>788</v>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>1.4 [1.2,1.7]</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
         <is>
           <t>1.4 [1.2,1.7]</t>
         </is>
@@ -2747,10 +2447,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A32:A37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Results with just one cohort
</commit_message>
<xml_diff>
--- a/results/table1/coh_1.xlsx
+++ b/results/table1/coh_1.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,10 +519,10 @@
       <c r="B4" s="1" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>5509</v>
+        <v>2448</v>
       </c>
       <c r="E4" t="n">
-        <v>11090</v>
+        <v>10603</v>
       </c>
     </row>
     <row r="5">
@@ -541,12 +541,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1528 (27.7)</t>
+          <t>1015 (41.5)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4208 (37.9)</t>
+          <t>3965 (37.4)</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1335 (24.2)</t>
+          <t>596 (24.3)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2672 (24.1)</t>
+          <t>2561 (24.2)</t>
         </is>
       </c>
     </row>
@@ -579,12 +579,12 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1453 (26.4)</t>
+          <t>507 (20.7)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2494 (22.5)</t>
+          <t>2420 (22.8)</t>
         </is>
       </c>
     </row>
@@ -598,12 +598,12 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1193 (21.7)</t>
+          <t>330 (13.5)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1716 (15.5)</t>
+          <t>1657 (15.6)</t>
         </is>
       </c>
     </row>
@@ -623,12 +623,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2357 (42.8)</t>
+          <t>1170 (47.8)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4654 (42.0)</t>
+          <t>4450 (42.0)</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2175 (39.5)</t>
+          <t>932 (38.1)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5630 (50.8)</t>
+          <t>5370 (50.6)</t>
         </is>
       </c>
     </row>
@@ -667,12 +667,12 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>624 (11.3)</t>
+          <t>342 (14.0)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>591 (5.3)</t>
+          <t>560 (5.3)</t>
         </is>
       </c>
     </row>
@@ -686,12 +686,12 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2710 (49.2)</t>
+          <t>1174 (48.0)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4869 (43.9)</t>
+          <t>4673 (44.1)</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1232 (22.4)</t>
+          <t>770 (31.5)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>515 (4.6)</t>
+          <t>490 (4.6)</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>408 (7.4)</t>
+          <t>196 (8.0)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1573 (14.2)</t>
+          <t>1545 (14.6)</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1903 (34.5)</t>
+          <t>805 (32.9)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4633 (41.8)</t>
+          <t>4481 (42.3)</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1308 (23.7)</t>
+          <t>434 (17.7)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2075 (18.7)</t>
+          <t>1762 (16.6)</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1716 (31.1)</t>
+          <t>650 (26.6)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3048 (27.5)</t>
+          <t>2667 (25.2)</t>
         </is>
       </c>
     </row>
@@ -836,12 +836,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3230 (58.6)</t>
+          <t>1207 (49.3)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5698 (51.4)</t>
+          <t>5398 (50.9)</t>
         </is>
       </c>
     </row>
@@ -861,12 +861,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>451 (8.2)</t>
+          <t>227 (9.3)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>540 (4.9)</t>
+          <t>494 (4.7)</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2555 (46.4)</t>
+          <t>999 (40.8)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5333 (48.1)</t>
+          <t>5074 (47.9)</t>
         </is>
       </c>
     </row>
@@ -911,12 +911,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3675 (66.7)</t>
+          <t>1392 (56.9)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6715 (60.6)</t>
+          <t>6318 (59.6)</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>824 (15.0)</t>
+          <t>371 (15.2)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1159 (10.5)</t>
+          <t>1027 (9.7)</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3049 (55.3)</t>
+          <t>1181 (48.2)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6313 (56.9)</t>
+          <t>5932 (55.9)</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3379 (61.3)</t>
+          <t>1502 (61.4)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6677 (60.2)</t>
+          <t>6318 (59.6)</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>641 (11.6)</t>
+          <t>256 (10.5)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1368 (12.3)</t>
+          <t>1296 (12.2)</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>5398 (98.0)</t>
+          <t>2385 (97.4)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10844 (97.8)</t>
+          <t>10357 (97.7)</t>
         </is>
       </c>
     </row>
@@ -1061,12 +1061,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3571 (64.8)</t>
+          <t>1704 (69.6)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>7269 (65.5)</t>
+          <t>6977 (65.8)</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1887 (34.3)</t>
+          <t>915 (37.4)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4054 (36.6)</t>
+          <t>3851 (36.3)</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1259 (22.9)</t>
+          <t>562 (23.0)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2748 (24.8)</t>
+          <t>2623 (24.7)</t>
         </is>
       </c>
     </row>
@@ -1136,12 +1136,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>66 (1.2)</t>
+          <t>34 (1.4)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>171 (1.5)</t>
+          <t>152 (1.4)</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1810 (32.9)</t>
+          <t>754 (30.8)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4304 (38.8)</t>
+          <t>4137 (39.0)</t>
         </is>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>4 (0.1)</t>
+          <t>3 (0.1)</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1205,12 +1205,12 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>32 (0.6)</t>
+          <t>19 (0.8)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>70 (0.6)</t>
+          <t>68 (0.6)</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1224,12 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>294 (5.3)</t>
+          <t>161 (6.6)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>549 (5.0)</t>
+          <t>532 (5.0)</t>
         </is>
       </c>
     </row>
@@ -1243,12 +1243,12 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>103 (1.9)</t>
+          <t>62 (2.5)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>196 (1.8)</t>
+          <t>185 (1.7)</t>
         </is>
       </c>
     </row>
@@ -1262,12 +1262,12 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>395 (7.2)</t>
+          <t>264 (10.8)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>486 (4.4)</t>
+          <t>461 (4.3)</t>
         </is>
       </c>
     </row>
@@ -1281,12 +1281,12 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4681 (85.0)</t>
+          <t>1939 (79.2)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9787 (88.3)</t>
+          <t>9355 (88.2)</t>
         </is>
       </c>
     </row>
@@ -1306,12 +1306,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>127 (2.3)</t>
+          <t>75 (3.1)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>312 (2.8)</t>
+          <t>300 (2.8)</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1844 (33.5)</t>
+          <t>986 (40.3)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3084 (27.8)</t>
+          <t>2962 (27.9)</t>
         </is>
       </c>
     </row>
@@ -1344,12 +1344,12 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3538 (64.2)</t>
+          <t>1387 (56.7)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>7694 (69.4)</t>
+          <t>7341 (69.2)</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1369,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>225 (4.1)</t>
+          <t>117 (4.8)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>496 (4.5)</t>
+          <t>472 (4.5)</t>
         </is>
       </c>
     </row>
@@ -1394,12 +1394,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>305 (5.5)</t>
+          <t>139 (5.7)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>523 (4.7)</t>
+          <t>507 (4.8)</t>
         </is>
       </c>
     </row>
@@ -1419,12 +1419,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>31 (0.6)</t>
+          <t>15 (0.6)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>88 (0.8)</t>
+          <t>84 (0.8)</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>9 (0.2)</t>
+          <t>2 (0.1)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>23 (0.2)</t>
+          <t>20 (0.2)</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>6 (0.1)</t>
+          <t>4 (0.2)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1490,12 +1490,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>64 [52,76]</t>
+          <t>64 [52,75]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>68 [58,79]</t>
+          <t>68 [58,78]</t>
         </is>
       </c>
     </row>
@@ -1507,16 +1507,16 @@
       </c>
       <c r="B47" s="1" t="inlineStr"/>
       <c r="C47" t="n">
-        <v>13216</v>
+        <v>10855</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5.79 [3.58,10.68]</t>
+          <t>5.23 [3.23,8.99]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5.79 [3.54,10.29]</t>
+          <t>5.38 [3.29,9.38]</t>
         </is>
       </c>
     </row>
@@ -1528,16 +1528,16 @@
       </c>
       <c r="B48" s="1" t="inlineStr"/>
       <c r="C48" t="n">
-        <v>3383</v>
+        <v>2196</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4.63 [2.96,9.00]</t>
+          <t>4.17 [2.83,7.71]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4.13 [2.83,7.46]</t>
+          <t>4.08 [2.79,7.17]</t>
         </is>
       </c>
     </row>
@@ -1549,16 +1549,16 @@
       </c>
       <c r="B49" s="1" t="inlineStr"/>
       <c r="C49" t="n">
-        <v>13216</v>
+        <v>10855</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>9.00 [5.00,18.00]</t>
+          <t>10.00 [6.00,19.00]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>11.00 [6.00,19.00]</t>
+          <t>11.00 [6.00,18.75]</t>
         </is>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="B50" s="1" t="inlineStr"/>
       <c r="C50" t="n">
-        <v>3383</v>
+        <v>2196</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1616,12 +1616,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>6 [4,9]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>5 [3,8]</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B53" s="1" t="inlineStr"/>
       <c r="C53" t="n">
-        <v>5621</v>
+        <v>4756</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="B54" s="1" t="inlineStr"/>
       <c r="C54" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="B55" s="1" t="inlineStr"/>
       <c r="C55" t="n">
-        <v>6262</v>
+        <v>5163</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1696,11 +1696,11 @@
       </c>
       <c r="B56" s="1" t="inlineStr"/>
       <c r="C56" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1 [1,4]</t>
+          <t>1 [1,3]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B57" s="1" t="inlineStr"/>
       <c r="C57" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1754,691 +1754,544 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>sofa_max_0_24h, median [Q1,Q3]</t>
+          <t>Fluids Volume (first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B59" s="1" t="inlineStr"/>
       <c r="C59" t="n">
-        <v>16</v>
+        <v>4731</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5.0 [3.0,8.0]</t>
+          <t>729 [246,1498]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5.0 [3.0,8.0]</t>
+          <t>650 [210,1463]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>respiratory_max_0_24h, median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B60" s="1" t="inlineStr"/>
       <c r="C60" t="n">
-        <v>16</v>
+        <v>309</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>2648 [994,5920]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>2369 [817,5431]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>coagulation_max_0_24h, median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B61" s="1" t="inlineStr"/>
       <c r="C61" t="n">
-        <v>16</v>
+        <v>309</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>506.2 [226.7,963.1]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>477.0 [204.8,905.2]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>liver_max_0_24h, median [Q1,Q3]</t>
+          <t>FiO2 (mean %, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B62" s="1" t="inlineStr"/>
       <c r="C62" t="n">
-        <v>16</v>
+        <v>7672</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.0 [0.0,0.0]</t>
+          <t>50 [40,60]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0.0 [0.0,0.0]</t>
+          <t>50 [42,65]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>cardiovascular_max_0_24h, median [Q1,Q3]</t>
+          <t>MV_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B63" s="1" t="inlineStr"/>
       <c r="C63" t="n">
-        <v>16</v>
+        <v>5341</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.0 [1.0,3.0]</t>
+          <t>39.0 [17.0,86.2]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.0 [1.0,3.0]</t>
+          <t>32.0 [15.0,76.0]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>cns_max_0_24h, median [Q1,Q3]</t>
+          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B64" s="1" t="inlineStr"/>
       <c r="C64" t="n">
-        <v>16</v>
+        <v>5341</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>0.30 [0.14,0.50]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>0.26 [0.13,0.45]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>renal_max_0_24h, median [Q1,Q3]</t>
+          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B65" s="1" t="inlineStr"/>
       <c r="C65" t="n">
-        <v>16</v>
+        <v>5341</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.0 [0.0,2.0]</t>
+          <t>2.0 [1.0,8.0]</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.0 [0.0,1.0]</t>
+          <t>3.0 [1.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (first 24h), median [Q1,Q3]</t>
+          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B66" s="1" t="inlineStr"/>
       <c r="C66" t="n">
-        <v>5744</v>
+        <v>11653</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>800 [250,1564]</t>
+          <t>16.0 [4.0,41.0]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>681 [221,1500]</t>
+          <t>25.0 [5.5,63.0]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
+          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B67" s="1" t="inlineStr"/>
       <c r="C67" t="n">
-        <v>357</v>
+        <v>5827</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3304 [1158,7044]</t>
+          <t>3.0 [1.0,12.0]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2546 [869,5885]</t>
+          <t>3.0 [1.0,10.0]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
+          <t>VP_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B68" s="1" t="inlineStr"/>
       <c r="C68" t="n">
-        <v>357</v>
+        <v>5827</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>549.5 [259.8,1016.1]</t>
+          <t>29.0 [10.0,65.0]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>487.9 [213.9,917.0]</t>
+          <t>29.0 [11.0,62.0]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>FiO2 (mean %, first 24h), median [Q1,Q3]</t>
+          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B69" s="1" t="inlineStr"/>
       <c r="C69" t="n">
-        <v>9234</v>
+        <v>5827</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>50 [40,62]</t>
+          <t>0.23 [0.08,0.48]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>50 [42,65]</t>
+          <t>0.25 [0.09,0.47]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>MV_time_abs_hours, median [Q1,Q3]</t>
+          <t>Respiratory Rate (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B70" s="1" t="inlineStr"/>
       <c r="C70" t="n">
-        <v>6209</v>
+        <v>24</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>45.0 [18.0,98.0]</t>
+          <t>19.4 [17.0,22.6]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>35.0 [15.0,86.0]</t>
+          <t>19.1 [16.8,22.0]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>Mean Blood Pressure (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B71" s="1" t="inlineStr"/>
       <c r="C71" t="n">
-        <v>6209</v>
+        <v>18</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.31 [0.15,0.53]</t>
+          <t>77.5 [71.1,85.4]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.27 [0.13,0.46]</t>
+          <t>74.7 [69.4,81.6]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B72" s="1" t="inlineStr"/>
       <c r="C72" t="n">
-        <v>6209</v>
+        <v>693</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2.0 [1.0,6.0]</t>
+          <t>36.9 [36.6,37.3]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3.0 [1.0,8.0]</t>
+          <t>36.9 [36.6,37.2]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>SpO2 (%, mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B73" s="1" t="inlineStr"/>
       <c r="C73" t="n">
-        <v>14616</v>
+        <v>19</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>20.0 [4.0,58.2]</t>
+          <t>98.0 [96.3,99.2]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>27.0 [6.0,69.0]</t>
+          <t>97.2 [95.8,98.6]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>Heart Rate (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B74" s="1" t="inlineStr"/>
       <c r="C74" t="n">
-        <v>7088</v>
+        <v>18</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3.0 [1.0,12.0]</t>
+          <t>87.5 [76.4,100.6]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3.0 [1.0,10.0]</t>
+          <t>85.8 [75.8,97.9]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>VP_time_abs_hours, median [Q1,Q3]</t>
+          <t>PaO2 (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B75" s="1" t="inlineStr"/>
       <c r="C75" t="n">
-        <v>7088</v>
+        <v>4014</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>34.0 [12.0,80.0]</t>
+          <t>88.5 [69.0,124.0]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>31.0 [11.0,68.0]</t>
+          <t>89.0 [72.0,118.0]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>PaCO2 (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B76" s="1" t="inlineStr"/>
       <c r="C76" t="n">
-        <v>7088</v>
+        <v>4014</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.26 [0.09,0.52]</t>
+          <t>44.0 [37.0,52.0]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>0.25 [0.09,0.48]</t>
+          <t>46.0 [39.0,53.0]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>Respiratory Rate (mean, first 24h), median [Q1,Q3]</t>
+          <t>pH (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B77" s="1" t="inlineStr"/>
       <c r="C77" t="n">
-        <v>28</v>
+        <v>2267</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>19.4 [17.0,22.5]</t>
+          <t>7.3 [7.2,7.4]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>19.1 [16.8,22.1]</t>
+          <t>7.3 [7.2,7.4]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>Mean Blood Pressure (mean, first 24h), median [Q1,Q3]</t>
+          <t>Glucose (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B78" s="1" t="inlineStr"/>
       <c r="C78" t="n">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>76.7 [70.8,84.4]</t>
+          <t>154.0 [122.0,218.0]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>74.7 [69.4,81.5]</t>
+          <t>147.0 [120.0,194.0]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
+          <t>Sodium (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B79" s="1" t="inlineStr"/>
       <c r="C79" t="n">
-        <v>899</v>
+        <v>27</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.3]</t>
+          <t>137.0 [134.0,140.0]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.2]</t>
+          <t>137.0 [134.0,140.0]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>SpO2 (%, mean, first 24h), median [Q1,Q3]</t>
+          <t>Potassium (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B80" s="1" t="inlineStr"/>
       <c r="C80" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>97.8 [96.2,99.0]</t>
+          <t>4.5 [4.1,5.2]</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>97.2 [95.8,98.6]</t>
+          <t>4.5 [4.1,5.0]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>Heart Rate (mean, first 24h), median [Q1,Q3]</t>
+          <t>Cortisol (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B81" s="1" t="inlineStr"/>
       <c r="C81" t="n">
-        <v>22</v>
+        <v>12719</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>86.7 [76.2,99.5]</t>
+          <t>19.0 [13.5,30.9]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>86.0 [75.9,98.2]</t>
+          <t>22.0 [12.5,33.9]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>PaO2 (min, first 24h), median [Q1,Q3]</t>
+          <t>Hemoglobin (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B82" s="1" t="inlineStr"/>
       <c r="C82" t="n">
-        <v>4762</v>
+        <v>1753</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>88.0 [70.0,123.0]</t>
+          <t>9.8 [8.2,11.4]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>88.0 [71.0,117.0]</t>
+          <t>10.0 [8.6,11.6]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>PaCO2 (max, first 24h), median [Q1,Q3]</t>
+          <t>Fibrinogen (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B83" s="1" t="inlineStr"/>
       <c r="C83" t="n">
-        <v>4762</v>
+        <v>8424</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>44.0 [38.0,52.0]</t>
+          <t>226.0 [153.0,364.0]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>46.0 [39.0,53.0]</t>
+          <t>228.5 [165.0,344.0]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>pH (min, first 24h), median [Q1,Q3]</t>
+          <t>INR (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B84" s="1" t="inlineStr"/>
       <c r="C84" t="n">
-        <v>2649</v>
+        <v>788</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>7.3 [7.2,7.4]</t>
+          <t>1.4 [1.2,1.7]</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
-        <is>
-          <t>7.3 [7.2,7.4]</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>Glucose (max, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B85" s="1" t="inlineStr"/>
-      <c r="C85" t="n">
-        <v>82</v>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>154.0 [123.0,209.0]</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>147.0 [120.0,194.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>Sodium (min, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B86" s="1" t="inlineStr"/>
-      <c r="C86" t="n">
-        <v>33</v>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>137.0 [134.0,140.0]</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>137.0 [134.0,140.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>Potassium (max, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B87" s="1" t="inlineStr"/>
-      <c r="C87" t="n">
-        <v>40</v>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>4.5 [4.1,5.1]</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>4.5 [4.1,5.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>Cortisol (min, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B88" s="1" t="inlineStr"/>
-      <c r="C88" t="n">
-        <v>16187</v>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>22.6 [14.2,35.0]</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>22.4 [12.5,35.5]</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="inlineStr">
-        <is>
-          <t>Hemoglobin (min, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B89" s="1" t="inlineStr"/>
-      <c r="C89" t="n">
-        <v>2238</v>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>10.0 [8.5,11.7]</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>10.0 [8.6,11.6]</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>Fibrinogen (min, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B90" s="1" t="inlineStr"/>
-      <c r="C90" t="n">
-        <v>10497</v>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>229.0 [159.0,346.0]</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>230.0 [165.0,349.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="inlineStr">
-        <is>
-          <t>INR (max, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B91" s="1" t="inlineStr"/>
-      <c r="C91" t="n">
-        <v>899</v>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>1.3 [1.2,1.7]</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
         <is>
           <t>1.4 [1.2,1.7]</t>
         </is>

</xml_diff>

<commit_message>
Fix race_nonwhite in data cleaning
</commit_message>
<xml_diff>
--- a/results/table1/coh_1.xlsx
+++ b/results/table1/coh_1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -519,10 +519,10 @@
       <c r="B4" s="1" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>2448</v>
+        <v>2553</v>
       </c>
       <c r="E4" t="n">
-        <v>10603</v>
+        <v>11113</v>
       </c>
     </row>
     <row r="5">
@@ -541,12 +541,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1015 (41.5)</t>
+          <t>1066 (41.8)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3965 (37.4)</t>
+          <t>4222 (38.0)</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>596 (24.3)</t>
+          <t>623 (24.4)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2561 (24.2)</t>
+          <t>2677 (24.1)</t>
         </is>
       </c>
     </row>
@@ -579,12 +579,12 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>507 (20.7)</t>
+          <t>526 (20.6)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2420 (22.8)</t>
+          <t>2496 (22.5)</t>
         </is>
       </c>
     </row>
@@ -598,12 +598,12 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>330 (13.5)</t>
+          <t>338 (13.2)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1657 (15.6)</t>
+          <t>1718 (15.5)</t>
         </is>
       </c>
     </row>
@@ -623,12 +623,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1170 (47.8)</t>
+          <t>1217 (47.7)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4450 (42.0)</t>
+          <t>4665 (42.0)</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>932 (38.1)</t>
+          <t>973 (38.1)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5370 (50.6)</t>
+          <t>5641 (50.8)</t>
         </is>
       </c>
     </row>
@@ -667,12 +667,12 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>342 (14.0)</t>
+          <t>357 (14.0)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>560 (5.3)</t>
+          <t>594 (5.3)</t>
         </is>
       </c>
     </row>
@@ -686,12 +686,12 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1174 (48.0)</t>
+          <t>1223 (47.9)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4673 (44.1)</t>
+          <t>4878 (43.9)</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>770 (31.5)</t>
+          <t>803 (31.5)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>490 (4.6)</t>
+          <t>518 (4.7)</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>196 (8.0)</t>
+          <t>200 (7.8)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1545 (14.6)</t>
+          <t>1576 (14.2)</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>805 (32.9)</t>
+          <t>835 (32.7)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4481 (42.3)</t>
+          <t>4639 (41.7)</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>434 (17.7)</t>
+          <t>503 (19.7)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1762 (16.6)</t>
+          <t>2082 (18.7)</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>650 (26.6)</t>
+          <t>726 (28.4)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2667 (25.2)</t>
+          <t>3055 (27.5)</t>
         </is>
       </c>
     </row>
@@ -836,12 +836,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1207 (49.3)</t>
+          <t>1282 (50.2)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5398 (50.9)</t>
+          <t>5712 (51.4)</t>
         </is>
       </c>
     </row>
@@ -861,12 +861,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>227 (9.3)</t>
+          <t>244 (9.6)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>494 (4.7)</t>
+          <t>541 (4.9)</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>999 (40.8)</t>
+          <t>1070 (41.9)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5074 (47.9)</t>
+          <t>5342 (48.1)</t>
         </is>
       </c>
     </row>
@@ -911,12 +911,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1392 (56.9)</t>
+          <t>1489 (58.3)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6318 (59.6)</t>
+          <t>6731 (60.6)</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>371 (15.2)</t>
+          <t>415 (16.3)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1027 (9.7)</t>
+          <t>1165 (10.5)</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1181 (48.2)</t>
+          <t>1275 (49.9)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5932 (55.9)</t>
+          <t>6324 (56.9)</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1502 (61.4)</t>
+          <t>1582 (62.0)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6318 (59.6)</t>
+          <t>6691 (60.2)</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>256 (10.5)</t>
+          <t>279 (10.9)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1296 (12.2)</t>
+          <t>1370 (12.3)</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2385 (97.4)</t>
+          <t>2490 (97.5)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10357 (97.7)</t>
+          <t>10866 (97.8)</t>
         </is>
       </c>
     </row>
@@ -1061,12 +1061,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1704 (69.6)</t>
+          <t>1782 (69.8)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>6977 (65.8)</t>
+          <t>7281 (65.5)</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>915 (37.4)</t>
+          <t>955 (37.4)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3851 (36.3)</t>
+          <t>4064 (36.6)</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>562 (23.0)</t>
+          <t>584 (22.9)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2623 (24.7)</t>
+          <t>2754 (24.8)</t>
         </is>
       </c>
     </row>
@@ -1136,12 +1136,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>34 (1.4)</t>
+          <t>35 (1.4)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>152 (1.4)</t>
+          <t>171 (1.5)</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>754 (30.8)</t>
+          <t>784 (30.7)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4137 (39.0)</t>
+          <t>4313 (38.8)</t>
         </is>
       </c>
     </row>
@@ -1205,12 +1205,12 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>19 (0.8)</t>
+          <t>20 (0.8)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>68 (0.6)</t>
+          <t>70 (0.6)</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1224,12 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>161 (6.6)</t>
+          <t>168 (6.6)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>532 (5.0)</t>
+          <t>549 (4.9)</t>
         </is>
       </c>
     </row>
@@ -1243,12 +1243,12 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>62 (2.5)</t>
+          <t>66 (2.6)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>185 (1.7)</t>
+          <t>197 (1.8)</t>
         </is>
       </c>
     </row>
@@ -1262,12 +1262,12 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>264 (10.8)</t>
+          <t>278 (10.9)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>461 (4.3)</t>
+          <t>490 (4.4)</t>
         </is>
       </c>
     </row>
@@ -1281,12 +1281,12 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1939 (79.2)</t>
+          <t>2018 (79.0)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9355 (88.2)</t>
+          <t>9805 (88.2)</t>
         </is>
       </c>
     </row>
@@ -1306,12 +1306,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>75 (3.1)</t>
+          <t>76 (3.0)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>300 (2.8)</t>
+          <t>314 (2.8)</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>986 (40.3)</t>
+          <t>1022 (40.0)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2962 (27.9)</t>
+          <t>3090 (27.8)</t>
         </is>
       </c>
     </row>
@@ -1344,12 +1344,12 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1387 (56.7)</t>
+          <t>1455 (57.0)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>7341 (69.2)</t>
+          <t>7709 (69.4)</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1369,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>117 (4.8)</t>
+          <t>120 (4.7)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>472 (4.5)</t>
+          <t>499 (4.5)</t>
         </is>
       </c>
     </row>
@@ -1394,12 +1394,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>139 (5.7)</t>
+          <t>146 (5.7)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>507 (4.8)</t>
+          <t>523 (4.7)</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>84 (0.8)</t>
+          <t>88 (0.8)</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>20 (0.2)</t>
+          <t>23 (0.2)</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>68 [58,78]</t>
+          <t>68 [58,79]</t>
         </is>
       </c>
     </row>
@@ -1507,16 +1507,16 @@
       </c>
       <c r="B47" s="1" t="inlineStr"/>
       <c r="C47" t="n">
-        <v>10855</v>
+        <v>11081</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5.23 [3.23,8.99]</t>
+          <t>5.46 [3.46,9.94]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5.38 [3.29,9.38]</t>
+          <t>5.79 [3.54,10.29]</t>
         </is>
       </c>
     </row>
@@ -1528,16 +1528,16 @@
       </c>
       <c r="B48" s="1" t="inlineStr"/>
       <c r="C48" t="n">
-        <v>2196</v>
+        <v>2585</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4.17 [2.83,7.71]</t>
+          <t>4.23 [2.88,8.04]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4.08 [2.79,7.17]</t>
+          <t>4.13 [2.83,7.48]</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B49" s="1" t="inlineStr"/>
       <c r="C49" t="n">
-        <v>10855</v>
+        <v>11081</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>11.00 [6.00,18.75]</t>
+          <t>11.00 [6.00,19.00]</t>
         </is>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="B50" s="1" t="inlineStr"/>
       <c r="C50" t="n">
-        <v>2196</v>
+        <v>2585</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1616,12 +1616,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
+          <t>6 [4,9]</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
           <t>6 [4,8]</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>5 [3,8]</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B53" s="1" t="inlineStr"/>
       <c r="C53" t="n">
-        <v>4756</v>
+        <v>4933</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="B54" s="1" t="inlineStr"/>
       <c r="C54" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="B55" s="1" t="inlineStr"/>
       <c r="C55" t="n">
-        <v>5163</v>
+        <v>5308</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B56" s="1" t="inlineStr"/>
       <c r="C56" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B57" s="1" t="inlineStr"/>
       <c r="C57" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1759,16 +1759,16 @@
       </c>
       <c r="B59" s="1" t="inlineStr"/>
       <c r="C59" t="n">
-        <v>4731</v>
+        <v>4942</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>729 [246,1498]</t>
+          <t>748 [250,1500]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>650 [210,1463]</t>
+          <t>681 [220,1500]</t>
         </is>
       </c>
     </row>
@@ -1780,16 +1780,16 @@
       </c>
       <c r="B60" s="1" t="inlineStr"/>
       <c r="C60" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2648 [994,5920]</t>
+          <t>2915 [1043,6446]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2369 [817,5431]</t>
+          <t>2546 [870,5886]</t>
         </is>
       </c>
     </row>
@@ -1801,16 +1801,16 @@
       </c>
       <c r="B61" s="1" t="inlineStr"/>
       <c r="C61" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>506.2 [226.7,963.1]</t>
+          <t>521.7 [240.1,984.1]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>477.0 [204.8,905.2]</t>
+          <t>487.9 [213.9,917.1]</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="B62" s="1" t="inlineStr"/>
       <c r="C62" t="n">
-        <v>7672</v>
+        <v>7992</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1843,16 +1843,16 @@
       </c>
       <c r="B63" s="1" t="inlineStr"/>
       <c r="C63" t="n">
-        <v>5341</v>
+        <v>5446</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>39.0 [17.0,86.2]</t>
+          <t>43.0 [18.0,97.0]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>32.0 [15.0,76.0]</t>
+          <t>35.0 [15.0,86.0]</t>
         </is>
       </c>
     </row>
@@ -1864,16 +1864,16 @@
       </c>
       <c r="B64" s="1" t="inlineStr"/>
       <c r="C64" t="n">
-        <v>5341</v>
+        <v>5446</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.30 [0.14,0.50]</t>
+          <t>0.31 [0.15,0.52]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.26 [0.13,0.45]</t>
+          <t>0.27 [0.13,0.46]</t>
         </is>
       </c>
     </row>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B65" s="1" t="inlineStr"/>
       <c r="C65" t="n">
-        <v>5341</v>
+        <v>5446</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1906,16 +1906,16 @@
       </c>
       <c r="B66" s="1" t="inlineStr"/>
       <c r="C66" t="n">
-        <v>11653</v>
+        <v>12086</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>16.0 [4.0,41.0]</t>
+          <t>18.0 [4.0,48.5]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>25.0 [5.5,63.0]</t>
+          <t>27.0 [6.0,69.0]</t>
         </is>
       </c>
     </row>
@@ -1927,11 +1927,11 @@
       </c>
       <c r="B67" s="1" t="inlineStr"/>
       <c r="C67" t="n">
-        <v>5827</v>
+        <v>5950</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3.0 [1.0,12.0]</t>
+          <t>3.0 [1.0,13.0]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -1948,16 +1948,16 @@
       </c>
       <c r="B68" s="1" t="inlineStr"/>
       <c r="C68" t="n">
-        <v>5827</v>
+        <v>5950</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>29.0 [10.0,65.0]</t>
+          <t>32.0 [11.0,72.0]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>29.0 [11.0,62.0]</t>
+          <t>31.0 [11.0,68.0]</t>
         </is>
       </c>
     </row>
@@ -1969,16 +1969,16 @@
       </c>
       <c r="B69" s="1" t="inlineStr"/>
       <c r="C69" t="n">
-        <v>5827</v>
+        <v>5950</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.23 [0.08,0.48]</t>
+          <t>0.24 [0.08,0.49]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.25 [0.09,0.47]</t>
+          <t>0.25 [0.09,0.48]</t>
         </is>
       </c>
     </row>
@@ -1990,16 +1990,16 @@
       </c>
       <c r="B70" s="1" t="inlineStr"/>
       <c r="C70" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>19.4 [17.0,22.6]</t>
+          <t>19.5 [17.0,22.7]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>19.1 [16.8,22.0]</t>
+          <t>19.1 [16.8,22.1]</t>
         </is>
       </c>
     </row>
@@ -2011,16 +2011,16 @@
       </c>
       <c r="B71" s="1" t="inlineStr"/>
       <c r="C71" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>77.5 [71.1,85.4]</t>
+          <t>77.2 [71.0,85.2]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>74.7 [69.4,81.6]</t>
+          <t>74.7 [69.4,81.5]</t>
         </is>
       </c>
     </row>
@@ -2032,7 +2032,7 @@
       </c>
       <c r="B72" s="1" t="inlineStr"/>
       <c r="C72" t="n">
-        <v>693</v>
+        <v>720</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2053,11 +2053,11 @@
       </c>
       <c r="B73" s="1" t="inlineStr"/>
       <c r="C73" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>98.0 [96.3,99.2]</t>
+          <t>97.9 [96.3,99.2]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2074,16 +2074,16 @@
       </c>
       <c r="B74" s="1" t="inlineStr"/>
       <c r="C74" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>87.5 [76.4,100.6]</t>
+          <t>87.8 [76.6,100.8]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>85.8 [75.8,97.9]</t>
+          <t>86.0 [75.9,98.2]</t>
         </is>
       </c>
     </row>
@@ -2095,16 +2095,16 @@
       </c>
       <c r="B75" s="1" t="inlineStr"/>
       <c r="C75" t="n">
-        <v>4014</v>
+        <v>4140</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>88.5 [69.0,124.0]</t>
+          <t>88.0 [68.0,123.0]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>89.0 [72.0,118.0]</t>
+          <t>88.0 [71.0,117.0]</t>
         </is>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="B76" s="1" t="inlineStr"/>
       <c r="C76" t="n">
-        <v>4014</v>
+        <v>4140</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B77" s="1" t="inlineStr"/>
       <c r="C77" t="n">
-        <v>2267</v>
+        <v>2339</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2158,11 +2158,11 @@
       </c>
       <c r="B78" s="1" t="inlineStr"/>
       <c r="C78" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>154.0 [122.0,218.0]</t>
+          <t>155.0 [122.0,217.0]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="B79" s="1" t="inlineStr"/>
       <c r="C79" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="B80" s="1" t="inlineStr"/>
       <c r="C80" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2221,16 +2221,16 @@
       </c>
       <c r="B81" s="1" t="inlineStr"/>
       <c r="C81" t="n">
-        <v>12719</v>
+        <v>13311</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>19.0 [13.5,30.9]</t>
+          <t>22.2 [13.6,31.4]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>22.0 [12.5,33.9]</t>
+          <t>22.4 [12.5,35.6]</t>
         </is>
       </c>
     </row>
@@ -2242,11 +2242,11 @@
       </c>
       <c r="B82" s="1" t="inlineStr"/>
       <c r="C82" t="n">
-        <v>1753</v>
+        <v>1819</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>9.8 [8.2,11.4]</t>
+          <t>9.8 [8.3,11.4]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2263,16 +2263,16 @@
       </c>
       <c r="B83" s="1" t="inlineStr"/>
       <c r="C83" t="n">
-        <v>8424</v>
+        <v>8836</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>226.0 [153.0,364.0]</t>
+          <t>227.0 [153.0,361.0]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>228.5 [165.0,344.0]</t>
+          <t>230.0 [165.0,348.0]</t>
         </is>
       </c>
     </row>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="B84" s="1" t="inlineStr"/>
       <c r="C84" t="n">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
New cohort selection and running results
</commit_message>
<xml_diff>
--- a/results/table1/coh_1.xlsx
+++ b/results/table1/coh_1.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,10 +519,10 @@
       <c r="B4" s="1" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>2553</v>
+        <v>2236</v>
       </c>
       <c r="E4" t="n">
-        <v>11113</v>
+        <v>10477</v>
       </c>
     </row>
     <row r="5">
@@ -541,12 +541,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1066 (41.8)</t>
+          <t>895 (40.0)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4222 (38.0)</t>
+          <t>3938 (37.6)</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>623 (24.4)</t>
+          <t>562 (25.1)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2677 (24.1)</t>
+          <t>2523 (24.1)</t>
         </is>
       </c>
     </row>
@@ -579,12 +579,12 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>526 (20.6)</t>
+          <t>471 (21.1)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2496 (22.5)</t>
+          <t>2374 (22.7)</t>
         </is>
       </c>
     </row>
@@ -598,12 +598,12 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>338 (13.2)</t>
+          <t>308 (13.8)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1718 (15.5)</t>
+          <t>1642 (15.7)</t>
         </is>
       </c>
     </row>
@@ -623,12 +623,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1217 (47.7)</t>
+          <t>1068 (47.8)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4665 (42.0)</t>
+          <t>4418 (42.2)</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>973 (38.1)</t>
+          <t>793 (35.5)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5641 (50.8)</t>
+          <t>5218 (49.8)</t>
         </is>
       </c>
     </row>
@@ -667,12 +667,12 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>357 (14.0)</t>
+          <t>332 (14.8)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>594 (5.3)</t>
+          <t>577 (5.5)</t>
         </is>
       </c>
     </row>
@@ -686,12 +686,12 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1223 (47.9)</t>
+          <t>1111 (49.7)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4878 (43.9)</t>
+          <t>4682 (44.7)</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>803 (31.5)</t>
+          <t>739 (33.1)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>518 (4.7)</t>
+          <t>478 (4.6)</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>200 (7.8)</t>
+          <t>192 (8.6)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1576 (14.2)</t>
+          <t>1517 (14.5)</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>835 (32.7)</t>
+          <t>742 (33.2)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4639 (41.7)</t>
+          <t>4433 (42.3)</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>503 (19.7)</t>
+          <t>419 (18.7)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2082 (18.7)</t>
+          <t>1902 (18.2)</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>726 (28.4)</t>
+          <t>609 (27.2)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3055 (27.5)</t>
+          <t>2794 (26.7)</t>
         </is>
       </c>
     </row>
@@ -836,12 +836,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1282 (50.2)</t>
+          <t>1153 (51.6)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5712 (51.4)</t>
+          <t>5427 (51.8)</t>
         </is>
       </c>
     </row>
@@ -861,12 +861,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>244 (9.6)</t>
+          <t>63 (2.8)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>541 (4.9)</t>
+          <t>276 (2.6)</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1070 (41.9)</t>
+          <t>923 (41.3)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5342 (48.1)</t>
+          <t>5008 (47.8)</t>
         </is>
       </c>
     </row>
@@ -911,12 +911,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1489 (58.3)</t>
+          <t>1331 (59.5)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6731 (60.6)</t>
+          <t>6392 (61.0)</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>415 (16.3)</t>
+          <t>159 (7.1)</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1165 (10.5)</t>
+          <t>723 (6.9)</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1275 (49.9)</t>
+          <t>1108 (49.6)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6324 (56.9)</t>
+          <t>5941 (56.7)</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1582 (62.0)</t>
+          <t>1376 (61.5)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6691 (60.2)</t>
+          <t>6270 (59.8)</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>279 (10.9)</t>
+          <t>241 (10.8)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1370 (12.3)</t>
+          <t>1290 (12.3)</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2490 (97.5)</t>
+          <t>2185 (97.7)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10866 (97.8)</t>
+          <t>10245 (97.8)</t>
         </is>
       </c>
     </row>
@@ -1061,12 +1061,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1782 (69.8)</t>
+          <t>1489 (66.6)</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>7281 (65.5)</t>
+          <t>6718 (64.1)</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>955 (37.4)</t>
+          <t>774 (34.6)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4064 (36.6)</t>
+          <t>3677 (35.1)</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>584 (22.9)</t>
+          <t>530 (23.7)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2754 (24.8)</t>
+          <t>2586 (24.7)</t>
         </is>
       </c>
     </row>
@@ -1136,12 +1136,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>35 (1.4)</t>
+          <t>30 (1.3)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>171 (1.5)</t>
+          <t>165 (1.6)</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>784 (30.7)</t>
+          <t>634 (28.4)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4313 (38.8)</t>
+          <t>3964 (37.8)</t>
         </is>
       </c>
     </row>
@@ -1205,12 +1205,12 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>20 (0.8)</t>
+          <t>21 (0.9)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>70 (0.6)</t>
+          <t>70 (0.7)</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1224,12 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>168 (6.6)</t>
+          <t>178 (8.0)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>549 (4.9)</t>
+          <t>559 (5.3)</t>
         </is>
       </c>
     </row>
@@ -1237,37 +1237,43 @@
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>Absent</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>66 (2.6)</t>
+          <t>2034 (91.0)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>197 (1.8)</t>
+          <t>9846 (94.0)</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n"/>
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Diabetes Type, n (%)</t>
+        </is>
+      </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr"/>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>278 (10.9)</t>
+          <t>48 (2.1)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>490 (4.4)</t>
+          <t>266 (2.5)</t>
         </is>
       </c>
     </row>
@@ -1275,88 +1281,94 @@
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2018 (79.0)</t>
+          <t>842 (37.7)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>9805 (88.2)</t>
+          <t>2782 (26.6)</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Diabetes Type, n (%)</t>
-        </is>
-      </c>
+      <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>1346 (60.2)</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>7429 (70.9)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Connective Tissue Disease, n (%)</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>76 (3.0)</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>314 (2.8)</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1022 (40.0)</t>
+          <t>97 (4.3)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3090 (27.8)</t>
+          <t>450 (4.3)</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n"/>
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Pneumonia, n (%)</t>
+        </is>
+      </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>Absent</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1455 (57.0)</t>
+          <t>129 (5.8)</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>7709 (69.4)</t>
+          <t>499 (4.8)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Connective Tissue Disease, n (%)</t>
+          <t>Urinary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr">
@@ -1369,19 +1381,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>120 (4.7)</t>
+          <t>15 (0.7)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>499 (4.5)</t>
+          <t>86 (0.8)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Pneumonia, n (%)</t>
+          <t>Biliary Tract Infection, n (%)</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr">
@@ -1394,19 +1406,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>146 (5.7)</t>
+          <t>2 (0.1)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>523 (4.7)</t>
+          <t>22 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Urinary Tract Infection, n (%)</t>
+          <t>Skin Infection, n (%)</t>
         </is>
       </c>
       <c r="B43" s="1" t="inlineStr">
@@ -1419,267 +1431,259 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15 (0.6)</t>
+          <t>3 (0.1)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>88 (0.8)</t>
+          <t>21 (0.2)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Biliary Tract Infection, n (%)</t>
-        </is>
-      </c>
-      <c r="B44" s="1" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+          <t>Age, median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr"/>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2 (0.1)</t>
+          <t>64 [52,76]</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>23 (0.2)</t>
+          <t>68 [57,79]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Skin Infection, n (%)</t>
-        </is>
-      </c>
-      <c r="B45" s="1" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr"/>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>10392</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4 (0.2)</t>
+          <t>5.50 [3.50,9.94]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>21 (0.2)</t>
+          <t>5.79 [3.50,10.17]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Age, median [Q1,Q3]</t>
+          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B46" s="1" t="inlineStr"/>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>2321</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>64 [52,75]</t>
+          <t>4.25 [2.88,8.13]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>68 [58,79]</t>
+          <t>4.13 [2.79,7.48]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if deceased), median [Q1,Q3]</t>
+          <t>Hospital LOS (days, if deceased), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B47" s="1" t="inlineStr"/>
       <c r="C47" t="n">
-        <v>11081</v>
+        <v>10392</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5.46 [3.46,9.94]</t>
+          <t>10.00 [6.00,19.00]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5.79 [3.54,10.29]</t>
+          <t>11.00 [6.00,18.00]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>ICU LOS (days, if survived), median [Q1,Q3]</t>
+          <t>Hospital LOS (days, if survived), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B48" s="1" t="inlineStr"/>
       <c r="C48" t="n">
-        <v>2585</v>
+        <v>2321</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4.23 [2.88,8.04]</t>
+          <t>12.00 [7.00,20.00]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4.13 [2.83,7.48]</t>
+          <t>11.00 [7.00,18.00]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Hospital LOS (days, if deceased), median [Q1,Q3]</t>
+          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B49" s="1" t="inlineStr"/>
       <c r="C49" t="n">
-        <v>11081</v>
+        <v>0</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>10.00 [6.00,19.00]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>11.00 [6.00,19.00]</t>
+          <t>6 [4,8]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Hospital LOS (days, if survived), median [Q1,Q3]</t>
+          <t>SOFA Score (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B50" s="1" t="inlineStr"/>
       <c r="C50" t="n">
-        <v>2585</v>
+        <v>0</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12.00 [7.00,20.00]</t>
+          <t>5 [3,8]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>11.00 [7.00,18.00]</t>
+          <t>5 [3,8]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Charlson Comorbidity Index, median [Q1,Q3]</t>
+          <t>SOFA: Respiratory (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B51" s="1" t="inlineStr"/>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>4492</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>2 [1,3]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>2 [1,3]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>SOFA Score (admission), median [Q1,Q3]</t>
+          <t>SOFA: Coagulation (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B52" s="1" t="inlineStr"/>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>6 [4,9]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>6 [4,8]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Respiratory (admission), median [Q1,Q3]</t>
+          <t>SOFA: Liver (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B53" s="1" t="inlineStr"/>
       <c r="C53" t="n">
-        <v>4933</v>
+        <v>5003</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2 [1,3]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2 [1,3]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Coagulation (admission), median [Q1,Q3]</t>
+          <t>SOFA: Cardiovascular (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B54" s="1" t="inlineStr"/>
       <c r="C54" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>1 [1,3]</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>1 [1,3]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Liver (admission), median [Q1,Q3]</t>
+          <t>SOFA: CNS (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B55" s="1" t="inlineStr"/>
       <c r="C55" t="n">
-        <v>5308</v>
+        <v>26</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>0 [0,2]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1691,607 +1695,565 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Cardiovascular (admission), median [Q1,Q3]</t>
+          <t>SOFA: Renal (admission), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B56" s="1" t="inlineStr"/>
       <c r="C56" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1 [1,3]</t>
+          <t>1 [0,2]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1 [1,3]</t>
+          <t>0 [0,1]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>SOFA: CNS (admission), median [Q1,Q3]</t>
+          <t>Fluids Volume (first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B57" s="1" t="inlineStr"/>
       <c r="C57" t="n">
-        <v>27</v>
+        <v>4530</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>833 [250,1553]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0 [0,1]</t>
+          <t>700 [227,1505]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>SOFA: Renal (admission), median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B58" s="1" t="inlineStr"/>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1 [0,2]</t>
+          <t>3103 [1104,6587]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1 [0,2]</t>
+          <t>2584 [891,5938]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (first 24h), median [Q1,Q3]</t>
+          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B59" s="1" t="inlineStr"/>
       <c r="C59" t="n">
-        <v>4942</v>
+        <v>283</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>748 [250,1500]</t>
+          <t>546.0 [253.2,1024.4]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>681 [220,1500]</t>
+          <t>491.8 [216.4,926.8]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay), median [Q1,Q3]</t>
+          <t>FiO2 (mean %, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B60" s="1" t="inlineStr"/>
       <c r="C60" t="n">
-        <v>310</v>
+        <v>7330</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2915 [1043,6446]</t>
+          <t>50 [40,60]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2546 [870,5886]</t>
+          <t>50 [42,65]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Fluids Volume (whole stay, normalized by ICU LOS), median [Q1,Q3]</t>
+          <t>MV_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B61" s="1" t="inlineStr"/>
       <c r="C61" t="n">
-        <v>310</v>
+        <v>4990</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>521.7 [240.1,984.1]</t>
+          <t>42.0 [18.0,93.0]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>487.9 [213.9,917.1]</t>
+          <t>34.0 [15.0,85.0]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>FiO2 (mean %, first 24h), median [Q1,Q3]</t>
+          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B62" s="1" t="inlineStr"/>
       <c r="C62" t="n">
-        <v>7992</v>
+        <v>4990</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>50 [40,60]</t>
+          <t>0.31 [0.14,0.51]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>50 [42,65]</t>
+          <t>0.27 [0.13,0.46]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>MV_time_abs_hours, median [Q1,Q3]</t>
+          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B63" s="1" t="inlineStr"/>
       <c r="C63" t="n">
-        <v>5446</v>
+        <v>4990</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>43.0 [18.0,97.0]</t>
+          <t>2.0 [1.0,8.0]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>35.0 [15.0,86.0]</t>
+          <t>3.0 [1.0,8.0]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>MV Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B64" s="1" t="inlineStr"/>
       <c r="C64" t="n">
-        <v>5446</v>
+        <v>11831</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.31 [0.15,0.52]</t>
+          <t>41.0 [9.5,97.0]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.27 [0.13,0.46]</t>
+          <t>43.0 [11.0,97.0]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>MV_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B65" s="1" t="inlineStr"/>
       <c r="C65" t="n">
-        <v>5446</v>
+        <v>5554</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2.0 [1.0,8.0]</t>
+          <t>4.0 [1.0,14.0]</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>3.0 [1.0,8.0]</t>
+          <t>3.0 [1.0,10.0]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>RRT_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>VP_time_abs_hours, median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B66" s="1" t="inlineStr"/>
       <c r="C66" t="n">
-        <v>12086</v>
+        <v>5554</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>18.0 [4.0,48.5]</t>
+          <t>29.0 [10.0,67.0]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>27.0 [6.0,69.0]</t>
+          <t>30.0 [11.0,67.0]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>VP_init_offset_abs_hours, median [Q1,Q3]</t>
+          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B67" s="1" t="inlineStr"/>
       <c r="C67" t="n">
-        <v>5950</v>
+        <v>5554</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3.0 [1.0,13.0]</t>
+          <t>0.22 [0.07,0.45]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>3.0 [1.0,10.0]</t>
+          <t>0.25 [0.09,0.47]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>VP_time_abs_hours, median [Q1,Q3]</t>
+          <t>Respiratory Rate (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B68" s="1" t="inlineStr"/>
       <c r="C68" t="n">
-        <v>5950</v>
+        <v>28</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>32.0 [11.0,72.0]</t>
+          <t>19.6 [17.1,22.9]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>31.0 [11.0,68.0]</t>
+          <t>19.1 [16.8,22.1]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Vasopressor Time (duration in the stay, % of ICU LOS), median [Q1,Q3]</t>
+          <t>Mean Blood Pressure (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B69" s="1" t="inlineStr"/>
       <c r="C69" t="n">
-        <v>5950</v>
+        <v>22</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.24 [0.08,0.49]</t>
+          <t>77.7 [71.5,85.5]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.25 [0.09,0.48]</t>
+          <t>74.8 [69.5,81.7]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>Respiratory Rate (mean, first 24h), median [Q1,Q3]</t>
+          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B70" s="1" t="inlineStr"/>
       <c r="C70" t="n">
-        <v>28</v>
+        <v>680</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>19.5 [17.0,22.7]</t>
+          <t>36.9 [36.6,37.3]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>19.1 [16.8,22.1]</t>
+          <t>36.9 [36.6,37.2]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>Mean Blood Pressure (mean, first 24h), median [Q1,Q3]</t>
+          <t>SpO2 (%, mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B71" s="1" t="inlineStr"/>
       <c r="C71" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>77.2 [71.0,85.2]</t>
+          <t>97.9 [96.3,99.1]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>74.7 [69.4,81.5]</t>
+          <t>97.2 [95.8,98.6]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>Temperature (mean, first 24h), median [Q1,Q3]</t>
+          <t>Heart Rate (mean, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B72" s="1" t="inlineStr"/>
       <c r="C72" t="n">
-        <v>720</v>
+        <v>22</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.3]</t>
+          <t>88.6 [77.1,101.3]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>36.9 [36.6,37.2]</t>
+          <t>86.1 [76.1,98.4]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>SpO2 (%, mean, first 24h), median [Q1,Q3]</t>
+          <t>PaO2 (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B73" s="1" t="inlineStr"/>
       <c r="C73" t="n">
-        <v>24</v>
+        <v>3752</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>97.9 [96.3,99.2]</t>
+          <t>89.0 [69.0,123.0]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>97.2 [95.8,98.6]</t>
+          <t>89.0 [71.0,117.0]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>Heart Rate (mean, first 24h), median [Q1,Q3]</t>
+          <t>PaCO2 (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B74" s="1" t="inlineStr"/>
       <c r="C74" t="n">
-        <v>22</v>
+        <v>3752</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>87.8 [76.6,100.8]</t>
+          <t>44.0 [37.0,52.0]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>86.0 [75.9,98.2]</t>
+          <t>46.0 [39.0,53.0]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>PaO2 (min, first 24h), median [Q1,Q3]</t>
+          <t>pH (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B75" s="1" t="inlineStr"/>
       <c r="C75" t="n">
-        <v>4140</v>
+        <v>2139</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>88.0 [68.0,123.0]</t>
+          <t>7.3 [7.2,7.4]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>88.0 [71.0,117.0]</t>
+          <t>7.3 [7.2,7.4]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>PaCO2 (max, first 24h), median [Q1,Q3]</t>
+          <t>Glucose (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B76" s="1" t="inlineStr"/>
       <c r="C76" t="n">
-        <v>4140</v>
+        <v>69</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>44.0 [37.0,52.0]</t>
+          <t>155.0 [123.0,216.0]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>46.0 [39.0,53.0]</t>
+          <t>147.0 [120.0,194.0]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>pH (min, first 24h), median [Q1,Q3]</t>
+          <t>Sodium (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B77" s="1" t="inlineStr"/>
       <c r="C77" t="n">
-        <v>2339</v>
+        <v>29</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>7.3 [7.2,7.4]</t>
+          <t>137.0 [134.0,140.0]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>7.3 [7.2,7.4]</t>
+          <t>137.0 [134.0,140.0]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>Glucose (max, first 24h), median [Q1,Q3]</t>
+          <t>Potassium (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B78" s="1" t="inlineStr"/>
       <c r="C78" t="n">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>155.0 [122.0,217.0]</t>
+          <t>4.5 [4.1,5.1]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>147.0 [120.0,194.0]</t>
+          <t>4.5 [4.1,4.9]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Sodium (min, first 24h), median [Q1,Q3]</t>
+          <t>Cortisol (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B79" s="1" t="inlineStr"/>
       <c r="C79" t="n">
-        <v>29</v>
+        <v>12393</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>137.0 [134.0,140.0]</t>
+          <t>22.5 [14.5,31.6]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>137.0 [134.0,140.0]</t>
+          <t>22.1 [12.3,35.2]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>Potassium (max, first 24h), median [Q1,Q3]</t>
+          <t>Hemoglobin (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B80" s="1" t="inlineStr"/>
       <c r="C80" t="n">
-        <v>36</v>
+        <v>1724</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4.5 [4.1,5.2]</t>
+          <t>10.0 [8.4,11.5]</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>4.5 [4.1,5.0]</t>
+          <t>10.1 [8.6,11.7]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>Cortisol (min, first 24h), median [Q1,Q3]</t>
+          <t>Fibrinogen (min, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B81" s="1" t="inlineStr"/>
       <c r="C81" t="n">
-        <v>13311</v>
+        <v>8167</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>22.2 [13.6,31.4]</t>
+          <t>224.0 [153.0,356.8]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>22.4 [12.5,35.6]</t>
+          <t>228.0 [164.0,343.0]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>Hemoglobin (min, first 24h), median [Q1,Q3]</t>
+          <t>INR (max, first 24h), median [Q1,Q3]</t>
         </is>
       </c>
       <c r="B82" s="1" t="inlineStr"/>
       <c r="C82" t="n">
-        <v>1819</v>
+        <v>754</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>9.8 [8.3,11.4]</t>
+          <t>1.4 [1.2,1.7]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
-        <is>
-          <t>10.0 [8.6,11.6]</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Fibrinogen (min, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B83" s="1" t="inlineStr"/>
-      <c r="C83" t="n">
-        <v>8836</v>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>227.0 [153.0,361.0]</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>230.0 [165.0,348.0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>INR (max, first 24h), median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B84" s="1" t="inlineStr"/>
-      <c r="C84" t="n">
-        <v>811</v>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>1.4 [1.2,1.7]</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
         <is>
           <t>1.4 [1.2,1.7]</t>
         </is>
@@ -2299,11 +2261,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A32:A35"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>